<commit_message>
Update before review 1
</commit_message>
<xml_diff>
--- a/ppt/references.xlsx
+++ b/ppt/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mini ke saath project\review 1\ppt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E4CE805-4723-4382-8315-7E8D329F7260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186E8ED0-735E-4534-AE0A-9D7296B1F93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F3AA150-F655-49E1-99B5-8356180D184D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t xml:space="preserve">Paper </t>
   </si>
@@ -52,13 +52,6 @@
 D. Arun Kumar, Student, Rajalakshmi Engineering College
 M. Arutselvan, Student, Rajalakshmi Engineering College
 S. Barath Ram, Student, Rajalakshmi Engineering College</t>
-  </si>
-  <si>
-    <t>A Survey on Chatbot Implementation
-in Health Care using NLTK</t>
-  </si>
-  <si>
-    <t>3, March 2020</t>
   </si>
   <si>
     <t>https://ijcsmc.com/docs/papers/March2020/V9I3202029.pdf</t>
@@ -85,14 +78,6 @@
 Maintenance Complexity: Keeping chatbot knowledge current requires resource-intensive maintenance.</t>
   </si>
   <si>
-    <t>The evaluation of chatbot as a tool
-for health literacy education among
-undergraduate students</t>
-  </si>
-  <si>
-    <t>2021 May 25</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8144870/</t>
   </si>
   <si>
@@ -121,22 +106,194 @@
   <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9536768/</t>
   </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9332458</t>
+  </si>
+  <si>
+    <t>Natural Language Processing and Its Applications in Machine Translation: A Diachronic Review</t>
+  </si>
+  <si>
+    <t>The Development and Use of Chatbots in Public Health : Scoping Review</t>
+  </si>
+  <si>
+    <t>Kai Jiang - College of Foreign Languages, Huazhong Agricultural University, Wuhan, China
+Xi Lu - Department of Common Required Courses, Hubei Institute of Fine Arts, Wuhan, China</t>
+  </si>
+  <si>
+    <t>IEEE</t>
+  </si>
+  <si>
+    <t>Accessibility: Chatbots provide 24/7 accessibility, allowing users to seek assistance or information at any time, which can be especially valuable for individuals with urgent health concerns.
+Scalability: Chatbots can handle a large number of users simultaneously, making them efficient tools for disseminating health information and resources, particularly during public health emergencies like the COVID-19 pandemic.
+Consistency: Chatbots can deliver consistent and evidence-based information, reducing the risk of misinformation that might occur with human interactions.
+Reduced Healthcare Costs: Chatbots can help in tasks like triage and symptom assessment, reducing the burden on healthcare facilities and potentially lowering healthcare costs.
+Anonymity: Users often feel more comfortable sharing sensitive health information with chatbots than with humans, which can be beneficial for mental health support or discussing sensitive issues.
+Education and Support: Chatbots can provide users with information about various health topics, promote healthy behaviors, and offer emotional support.</t>
+  </si>
+  <si>
+    <t>Limited Diagnostic Accuracy: Chatbots, especially those without advanced artificial intelligence (AI), may have limitations in accurately diagnosing medical conditions, which can lead to incorrect advice or reassurance.
+Lack of Empathy: While chatbots can simulate human-like interactions, they lack the empathy and emotional understanding that human healthcare providers can offer, which is crucial in certain healthcare contexts.
+Privacy Concerns: Chatbots require access to personal health information, raising concerns about data security and privacy breaches, especially if the data is not properly protected.
+Overreliance: Users may rely too heavily on chatbots for medical advice, potentially delaying seeking help from healthcare professionals when needed.
+Language and Communication Barriers: Users who are not proficient in the chatbot's language or those with disabilities may face challenges in effectively communicating with chatbots.
+Ethical Concerns: The use of chatbots for mental health support raises ethical questions about the appropriateness of using AI for sensitive issues and the potential for neglecting human support.
+User Experience Variability: User satisfaction with chatbots can vary widely based on factors like chatbot design, responsiveness, and the user's expectations.</t>
+  </si>
+  <si>
+    <t>Chatbot for Healthcare System Using Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9197833</t>
+  </si>
+  <si>
+    <t>An AI-Based Medical Chatbot Model for Infectious Disease Prediction</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9970731</t>
+  </si>
+  <si>
+    <t>https://ijacen.iraj.in/paper_detail.php?paper_id=18651</t>
+  </si>
+  <si>
+    <t>Institute of Research and Journals</t>
+  </si>
+  <si>
+    <t>A Survey on Chatbot Implementation in Health Care using NLTK</t>
+  </si>
+  <si>
+    <t>The evaluation of chatbot as a tool for health literacy education among undergraduate students</t>
+  </si>
+  <si>
+    <t>Lekha Athota - Amity University, Dubai, UAE
+Vinod Kumar Shukla - Amity University, Dubai, UAE
+Nitin Pandey - Amity University, Noida, UP, India
+Ajay Rana - Amity University Uttar Pradesh, Noida, India</t>
+  </si>
+  <si>
+    <t>http://www.iraj.in/journal/journal_file/journal_pdf/3-596-15734507561-6.pdf</t>
+  </si>
+  <si>
+    <t>Relevance: The topic of fake news detection using NLP and machine learning algorithms is highly relevant in today's digital age where misinformation is a significant concern.
+Comprehensive Research: The paper appears to offer a comprehensive exploration of the topic, including literature review, data collection, preprocessing, and implementation of various machine learning algorithms.
+Methodology: The paper outlines a clear methodology, including data preprocessing techniques like lemmatization and stemming, vectorization using TF-IDF, and the application of different machine learning algorithms.
+Comparative Analysis: The research paper provides a comparative analysis of the performance of different machine learning algorithms (Naive Bayes, SVM, Max Entropy) in fake news detection. This can be valuable for researchers and practitioners.
+Results: The inclusion of accuracy results for each algorithm before and after NLP techniques demonstrate the effectiveness of the proposed approach.
+References: The paper cites relevant prior research, enhancing its credibility and supporting the arguments made.</t>
+  </si>
+  <si>
+    <t>Lack of Detailed Explanation: The content provided here is an abstract, and while it gives an overview of the paper's contents, it lacks detailed explanations and in-depth analysis that would be present in the full paper.
+Data Sources: The paper mentions data collection but does not provide information on the sources of the dataset used. Transparency regarding data sources and potential biases is essential in research.
+Limited Context: Without the full paper, it's challenging to assess the context, limitations, and potential ethical considerations of the research.
+No Citations: The references section mentions some sources, but specific in-text citations are missing in this content snippet, making it difficult to identify the sources of the information presented.</t>
+  </si>
+  <si>
+    <t>News entity classification using NLP</t>
+  </si>
+  <si>
+    <t>Intelligent AI-based dialogue agent to enhance communication in organ transplant networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficient Communication Enhancement: The dialogue agent is designed to address communication deficiencies in organ transplant networks, which can potentially streamline the process and save lives.
+Automation: The system automates the process of answering user queries, making it more efficient and reducing delays caused by human communication gaps.
+Incorporates Advanced Technologies: It leverages technologies such as Natural Language Processing (NLP), Natural Language Understanding (NLU), and Natural Language Generation (NLG), along with Long Short-Term Memory (LSTM) neural networks and word embeddings like GloVe, which are cutting-edge in the field of AI.
+Web Scraping for Information Retrieval: The system can retrieve information from the web to provide more comprehensive answers to user queries, even if the information is not available in its initial training corpus.
+Multidomain Knowledge: The dialogue agent integrates knowledge from various domains, including authorized transplant centers, legal matters, general information, and NGO contact details, making it a valuable resource for users.
+</t>
+  </si>
+  <si>
+    <t>Data Limitation: The system's effectiveness heavily relies on the quality and quantity of data available in its training corpus. If the corpus lacks comprehensive information, it may not provide accurate answers.
+Training Complexity: Building and training the LSTM-based model, as well as collecting and preprocessing the training data, can be a complex and resource-intensive task.
+Maintenance: To ensure the system remains up-to-date and accurate, continuous monitoring and maintenance are required, especially when dealing with web scraping for information retrieval.
+Limited Contextual Understanding: While the system uses advanced NLP and LSTM models, it may still struggle with understanding nuanced or context-specific queries.
+Legal and Ethical Concerns: Dealing with sensitive topics like organ transplantation and legal matters requires adherence to strict ethical and legal standards. Ensuring compliance can be a challenge.
+Dependency on Web Search: The system relies on web search results to provide additional information. This dependency may lead to variations in the quality of answers based on the sources available on the web.</t>
+  </si>
+  <si>
+    <t>Lee Wilson PhD
+Mariana Marasoiu Mphil</t>
+  </si>
+  <si>
+    <t>Improved Accessibility: The chatbot provides users with easy access to medical information, including contact details for doctors and hospitals, which can be particularly helpful in emergencies or for individuals in remote areas.
+24/7 Support: Chatbots are available round-the-clock, offering users instant responses to their queries and eliminating the need to wait for business hours.
+Cost-Efficient: Implementing a chatbot can be cost-effective compared to maintaining a human workforce, particularly for handling a large volume of user inquiries.
+Reduced Stress: Users might feel more comfortable discussing their health concerns with a chatbot, potentially reducing the stress associated with talking to a human healthcare provider.
+Quick Response Time: Chatbots can respond to queries instantly, which is crucial in healthcare situations where timely information can be life-saving.
+Information Handling: Chatbots can efficiently handle large volumes of medical information, ensuring that users receive accurate responses to their questions.
+Training Model: The paper outlines the process of building a training model using TensorFlow and NLP, which can be valuable for developers looking to create similar applications.</t>
+  </si>
+  <si>
+    <t>Accuracy and Reliability: Chatbots are only as accurate as the data they are trained on. Inaccurate or outdated information can lead to incorrect responses, potentially causing harm or misinformation.
+Limited Scope: Chatbots like Kiwi are specialized in providing information about infectious diseases, which means they may not be suitable for addressing a broader range of medical concerns.
+Loss of Human Touch: While chatbots can be efficient, some users may prefer human interactions, especially when dealing with sensitive health issues.
+Technical Challenges: Developing and maintaining a chatbot, especially one that provides medical information, can be technically challenging and may require ongoing updates and improvements.
+Ethical and Privacy Concerns: Collecting and handling medical data, even in a chatbot, can raise ethical and privacy concerns, requiring strict adherence to data protection regulations.
+Language and Communication Limitations: Chatbots may struggle to understand complex or nuanced language, which can be a limitation in providing accurate responses to user queries.
+Dependency on Technology: Users relying solely on chatbots for medical information may become overly dependent on technology, potentially neglecting traditional healthcare resources.</t>
+  </si>
+  <si>
+    <t>International Journal for Research in Applied Science and Engineering Technology</t>
+  </si>
+  <si>
+    <t>Healthcare Chatbot using Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Anuj Patil</t>
+  </si>
+  <si>
+    <t>https://www.ijraset.com/best-journal/healthcare-chatbot-using-artificial-intelligence</t>
+  </si>
+  <si>
+    <t>Improved Accessibility: Chatbots provide users with 24/7 access to healthcare information and assistance, reducing the need to wait for appointments or healthcare providers' availability.
+Faster Responses: Chatbots can provide immediate responses to user queries, potentially helping users assess their health concerns more quickly.
+Cost-Efficiency: Chatbots can handle routine inquiries and administrative tasks, reducing the workload on healthcare staff and potentially lowering operational costs.
+Health Education: Chatbots can deliver health-related information and promote health literacy among users, helping them make informed decisions about their well-being.
+Remote Monitoring: Some medical chatbots can monitor users' health conditions remotely, which is especially valuable for patients with chronic illnesses.
+Privacy: Users may feel more comfortable discussing sensitive health issues with a chatbot than with a human, ensuring privacy and confidentiality.
+Scalability: Chatbots can handle a large volume of inquiries simultaneously, making them scalable for healthcare organizations.</t>
+  </si>
+  <si>
+    <t>Lack of Personalization: Chatbots may not provide the same level of personalized care as human healthcare providers, as they rely on algorithms and data patterns.
+Limited Medical Knowledge: Chatbots are only as knowledgeable as the data and algorithms they are built upon. They may not handle complex or rare medical conditions effectively.
+Misdiagnosis: There is a risk of chatbots providing inaccurate medical information or misdiagnosing health issues, potentially leading to harm if users rely solely on their advice.
+Ethical Concerns: Ensuring the ethical use of chatbots in healthcare, especially in areas like mental health or end-of-life care, can be challenging.
+Loss of Human Touch: Some patients may prefer human interaction and the empathy that healthcare providers can offer, which chatbots cannot replicate.
+Technical Issues: Chatbots may encounter technical glitches or errors that can frustrate users or lead to incorrect responses.
+Resistance to Adoption: Patients and healthcare providers may be resistant to adopting chatbot technology due to concerns about job displacement or mistrust of AI in healthcare.
+Data Privacy: Handling sensitive health data through chatbots requires robust security measures to protect user privacy, which can be challenging to implement effectively.</t>
+  </si>
+  <si>
+    <t>Sanjay Chakraborty
+Hrithik Paul
+Sayani Ghatak
+Saroj Kumar Pandey
+Ankit Kumar
+Kamred Udham Singh
+Mohd Asif Shah</t>
+  </si>
+  <si>
+    <t>Yaswanth Reddy
+Sri Charan
+Paul Aditya
+Ryan
+T. Mathu</t>
+  </si>
+  <si>
+    <t>Sumalatha M.R
+Aravind Rajagopalan
+Kaaviya Peranandam
+Vishwa S.S.K.M</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -146,6 +303,45 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,27 +381,52 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,24 +743,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F670B8-FD03-43DE-8F5A-BE20FDD54565}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.21875" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" customWidth="1"/>
-    <col min="6" max="6" width="51.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="72.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="25.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,69 +776,223 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="57.6">
+      <c r="A2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="15">
+        <v>44089</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="58.8" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="15">
+        <v>44228</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="103.2" customHeight="1">
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="15">
+        <v>44901</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="57.6" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15">
+        <v>43893</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="73.2" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15">
+        <v>44341</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="6" t="s">
+    <row r="7" spans="1:7" ht="72.599999999999994" customHeight="1">
+      <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15">
+        <v>44839</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
-        <v>21</v>
+    <row r="8" spans="1:7" ht="72.599999999999994" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="15">
+        <v>44775</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="61.8" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="15">
+        <v>43717</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="15">
+        <v>44786</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{471BBF12-9511-4668-A300-515886069339}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{6DC544FF-0406-487E-BD1E-EADFB60D28EA}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{471BBF12-9511-4668-A300-515886069339}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{6DC544FF-0406-487E-BD1E-EADFB60D28EA}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{47C5F2D9-DE1E-411B-A225-E35852390675}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{BD204D85-D42A-4E5E-ABA3-0AC48ACA6D0C}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{AD317454-2155-4886-A51A-398A57368E83}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{4B92B0E8-2A88-4289-9F98-BF61F34B403F}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{D0F6AC5A-81E5-4D18-B7AB-BC8F9E191F9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>